<commit_message>
excel image link update
</commit_message>
<xml_diff>
--- a/wiseProductCatalog/static/required_documents/wiseProductCatalogContentSheet.xlsx
+++ b/wiseProductCatalog/static/required_documents/wiseProductCatalogContentSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b845333281ed4adc/Desktop/Django/AutomationProductCatalogue/wiseProductCatalog/static/required_documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_F89D79EC0A87DA2B574E7B9617458C8D5FBF1985" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F7CEC55-ED1D-4618-B05C-79F5C867E33C}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_F89D79EC0A87DA2B574E7B9617458C8D5FBF1985" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F757E6C-F430-4477-896F-80D48436E432}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="121">
   <si>
     <t>VariableName</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/12Gdb9WIWbn4SVCujfF9iyygnHhcq4y3v/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>wiseSubProductsDefaultImage</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1a3zHSv6UtWz8grCGKEhn3gzV3exm89qg/view?usp=drive_link</t>
   </si>
 </sst>
 </file>
@@ -571,12 +577,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -584,9 +593,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -902,15 +908,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" style="13" customWidth="1"/>
     <col min="2" max="2" width="27.5546875" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
@@ -1210,21 +1216,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>9</v>
@@ -1233,29 +1241,40 @@
     <row r="30" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
       <c r="B30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DADD2B02-0A05-42F7-AA55-90C7E1755083}"/>
+    <hyperlink ref="B28" r:id="rId2" xr:uid="{2C149EC4-3367-497E-BD78-EDA6CBA42A9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1266,7 +1285,7 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1305,13 +1324,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="19" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1369,13 +1388,13 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="22" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1388,9 +1407,9 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="25"/>
-      <c r="C7" s="22"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1403,9 +1422,9 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="25"/>
-      <c r="C8" s="22"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1416,9 +1435,9 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="25"/>
-      <c r="C9" s="22"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1429,9 +1448,9 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="25"/>
-      <c r="C10" s="22"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1444,9 +1463,9 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="22"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1457,9 +1476,9 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="25"/>
-      <c r="C12" s="22"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1470,9 +1489,9 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="22"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1485,9 +1504,9 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="22"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1498,9 +1517,9 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1511,13 +1530,13 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="22" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1532,9 +1551,9 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1545,9 +1564,9 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1558,9 +1577,9 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
@@ -1571,13 +1590,13 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1592,9 +1611,9 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
@@ -1605,13 +1624,13 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="22" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1626,9 +1645,9 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
@@ -1640,10 +1659,10 @@
     </row>
     <row r="24" spans="1:7" s="3" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="19" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1760,10 +1779,10 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="22" t="s">
         <v>51</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1777,7 +1796,7 @@
     </row>
     <row r="34" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="20"/>
-      <c r="C34" s="22"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="2" t="s">
         <v>9</v>
       </c>
@@ -1791,7 +1810,7 @@
     </row>
     <row r="35" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="20"/>
-      <c r="C35" s="22"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="2" t="s">
         <v>9</v>
       </c>
@@ -1803,18 +1822,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="A6:A15"/>
-    <mergeCell ref="B6:B15"/>
-    <mergeCell ref="C6:C15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="C33:C35"/>
     <mergeCell ref="A22:A23"/>
@@ -1822,6 +1829,18 @@
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="B24:B32"/>
     <mergeCell ref="C24:C32"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="B6:B15"/>
+    <mergeCell ref="C6:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Some Changes of Video page
</commit_message>
<xml_diff>
--- a/wiseProductCatalog/static/required_documents/wiseProductCatalogContentSheet.xlsx
+++ b/wiseProductCatalog/static/required_documents/wiseProductCatalogContentSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b845333281ed4adc/Desktop/Django/AutomationProductCatalogue/wiseProductCatalog/static/required_documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Django\AutomationProductCatalogue\wiseProductCatalog\static\required_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="11_F89D79EC0A87DA2B574E7B9617458C8D5FBF1985" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2EC5163-3D81-4EA7-A3BD-B6F6EE2C45CE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560A82CC-2F88-4803-BF15-93EF63BE5D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="134">
   <si>
     <t>VariableName</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Sub Topics</t>
-  </si>
-  <si>
-    <t>sub Topicsvalue</t>
   </si>
   <si>
     <t>mainProductList1</t>
@@ -414,13 +411,31 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/19QzD23qyGDMp_lnZadzPWog8_c9anion/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>sub TopicsDescription</t>
+  </si>
+  <si>
+    <t>Making special occasions at our office even more memorable. We've created a smart Celebration Bot that automatically sends personalized emails and whatsapp messages for birthdays, weddings, and work anniversaries, using beautiful, customized templates. We believe that celebrating these milestones is a fantastic way to build a happy and supportive work environment. With the Celebration Bot, we're making it easy and enjoyable to show appreciation for each team member in a way that's as unique as they are. No more worrying about forgetting these significant dates, our bot takes care of it! Finds happiness in spreading smiles and creating a workplace where every birthday, wedding, work anniversary and special occasions are reasons to celebrate with a touch of personalized and delightful wishes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>sub TopicsTimeandcost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HR department can save a lot of time by just filling in the details of the employee at the starting of the year or whenever they require . Can enjoy the Bot making wishes for the employees on time on the date provided. Wishes on the employees special days can increase their bonds with the employers more. Which is priceless </t>
+  </si>
+  <si>
+    <t>sub Topics Features</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,6 +469,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -545,7 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -604,12 +631,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -619,12 +649,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -933,7 +965,7 @@
   </sheetPr>
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -957,346 +989,346 @@
     </row>
     <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>128</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C6" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C7" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="C9" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="3" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C10" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="C12" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="C14" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="C15" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="C21" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="C22" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="C23" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="C24" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="C25" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="C26" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>101</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>103</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1318,10 +1350,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,9 +1365,11 @@
     <col min="5" max="5" width="28.33203125" style="7" customWidth="1"/>
     <col min="6" max="6" width="64.21875" style="7" customWidth="1"/>
     <col min="7" max="7" width="36" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.44140625" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1352,365 +1386,379 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="B6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
+    <row r="7" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="23"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
+    <row r="8" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="23"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
+    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="23"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
+    <row r="10" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24"/>
       <c r="B10" s="26"/>
-      <c r="C10" s="23"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
+    <row r="12" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
       <c r="B12" s="26"/>
-      <c r="C12" s="23"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
+    <row r="13" spans="1:9" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
       <c r="B13" s="26"/>
-      <c r="C13" s="23"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
+    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>27</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="B20" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="C20" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>37</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" s="3" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1720,10 +1768,10 @@
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1733,10 +1781,10 @@
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1746,13 +1794,13 @@
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
       <c r="D27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G27" s="2"/>
     </row>
@@ -1761,13 +1809,13 @@
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
       <c r="D28" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -1776,10 +1824,10 @@
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
       <c r="D29" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1789,10 +1837,10 @@
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
       <c r="D30" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1802,10 +1850,10 @@
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1815,70 +1863,58 @@
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
       <c r="D32" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>50</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="2:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="21"/>
-      <c r="C34" s="23"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="21"/>
-      <c r="C35" s="23"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="A6:A15"/>
-    <mergeCell ref="B6:B15"/>
-    <mergeCell ref="C6:C15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="C33:C35"/>
     <mergeCell ref="A22:A23"/>
@@ -1886,6 +1922,18 @@
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="B24:B32"/>
     <mergeCell ref="C24:C32"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="B6:B15"/>
+    <mergeCell ref="C6:C15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{B69A256E-735F-4B5D-98AC-04A541926EBA}"/>

</xml_diff>